<commit_message>
fix "cheapest" local charges for a trip that was being generated through the creation of freight rates, but ONLY for Hong Kong Port
Former-commit-id: b793b5b13b1d27557c138dda19fb5dffbd9a12d8
</commit_message>
<xml_diff>
--- a/db/dummydata/speedtrans/speedtrans__freight_rates.xlsx
+++ b/db/dummydata/speedtrans/speedtrans__freight_rates.xlsx
@@ -5,7 +5,9 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$U$39</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -298,6 +300,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="26" width="15.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -415,7 +420,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -466,7 +471,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" hidden="1">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -510,7 +515,7 @@
         <v>60.0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
@@ -554,7 +559,7 @@
         <v>8.0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
@@ -598,7 +603,7 @@
         <v>33.0</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
@@ -642,7 +647,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
@@ -686,7 +691,7 @@
         <v>19.0</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1">
       <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
@@ -730,7 +735,7 @@
         <v>15.0</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="1">
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
@@ -774,7 +779,7 @@
         <v>23.0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
@@ -862,7 +867,7 @@
         <v>8.0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
@@ -906,7 +911,7 @@
         <v>45.0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
@@ -950,7 +955,7 @@
         <v>67.0</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
@@ -994,7 +999,7 @@
         <v>28.0</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="D16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>58.0</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="D17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>50.0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1126,7 +1131,7 @@
         <v>10.0</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1170,7 +1175,7 @@
         <v>27.0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1214,7 +1219,7 @@
         <v>14.0</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="D21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5.0</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1302,7 +1307,7 @@
         <v>12.0</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>5.0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1">
       <c r="D24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1390,7 +1395,7 @@
         <v>39.0</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1434,7 +1439,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="D26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1483,7 @@
         <v>19.0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1522,7 +1527,7 @@
         <v>29.0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="D28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1566,7 +1571,7 @@
         <v>78.0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="D29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1610,7 +1615,7 @@
         <v>40.0</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="D30" s="3" t="s">
         <v>21</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="D31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1698,7 +1703,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="D32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1742,7 +1747,7 @@
         <v>6.0</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="D33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>10.0</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="D34" s="3" t="s">
         <v>21</v>
       </c>
@@ -1830,7 +1835,7 @@
         <v>22.0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
@@ -1874,7 +1879,7 @@
         <v>38.0</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="D36" s="3" t="s">
         <v>21</v>
       </c>
@@ -1918,7 +1923,7 @@
         <v>51.0</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1">
       <c r="D37" s="3" t="s">
         <v>21</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>59.0</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="D38" s="3" t="s">
         <v>21</v>
       </c>
@@ -2006,7 +2011,7 @@
         <v>63.0</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1">
       <c r="D39" s="3" t="s">
         <v>21</v>
       </c>
@@ -2051,6 +2056,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$U$39">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Hong Kong"/>
+        <filter val="Kaohsiung"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>